<commit_message>
Changes of File path in Address Book
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5503" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5713" uniqueCount="1102">
   <si>
     <t>Sno</t>
   </si>
@@ -3194,6 +3194,132 @@
   </si>
   <si>
     <t>320018594709</t>
+  </si>
+  <si>
+    <t>320018608054</t>
+  </si>
+  <si>
+    <t>320018608065</t>
+  </si>
+  <si>
+    <t>320018608293</t>
+  </si>
+  <si>
+    <t>320018608319</t>
+  </si>
+  <si>
+    <t>320018608352</t>
+  </si>
+  <si>
+    <t>320018608374</t>
+  </si>
+  <si>
+    <t>320018608400</t>
+  </si>
+  <si>
+    <t>320018608422</t>
+  </si>
+  <si>
+    <t>320018608455</t>
+  </si>
+  <si>
+    <t>320018608477</t>
+  </si>
+  <si>
+    <t>320018608514</t>
+  </si>
+  <si>
+    <t>320018608536</t>
+  </si>
+  <si>
+    <t>320018608569</t>
+  </si>
+  <si>
+    <t>320018608580</t>
+  </si>
+  <si>
+    <t>320018608617</t>
+  </si>
+  <si>
+    <t>320018608639</t>
+  </si>
+  <si>
+    <t>320018608672</t>
+  </si>
+  <si>
+    <t>320018608694</t>
+  </si>
+  <si>
+    <t>320018608720</t>
+  </si>
+  <si>
+    <t>320018608742</t>
+  </si>
+  <si>
+    <t>320018608775</t>
+  </si>
+  <si>
+    <t>320018612013</t>
+  </si>
+  <si>
+    <t>320018612024</t>
+  </si>
+  <si>
+    <t>320018612057</t>
+  </si>
+  <si>
+    <t>320018612079</t>
+  </si>
+  <si>
+    <t>320018612116</t>
+  </si>
+  <si>
+    <t>320018612138</t>
+  </si>
+  <si>
+    <t>320018612160</t>
+  </si>
+  <si>
+    <t>320018612182</t>
+  </si>
+  <si>
+    <t>320018612219</t>
+  </si>
+  <si>
+    <t>320018612230</t>
+  </si>
+  <si>
+    <t>320018612274</t>
+  </si>
+  <si>
+    <t>320018612296</t>
+  </si>
+  <si>
+    <t>320018612322</t>
+  </si>
+  <si>
+    <t>320018612344</t>
+  </si>
+  <si>
+    <t>320018612377</t>
+  </si>
+  <si>
+    <t>320018612399</t>
+  </si>
+  <si>
+    <t>320018612436</t>
+  </si>
+  <si>
+    <t>320018612458</t>
+  </si>
+  <si>
+    <t>320018612480</t>
+  </si>
+  <si>
+    <t>320018612506</t>
+  </si>
+  <si>
+    <t>320018612539</t>
   </si>
 </sst>
 </file>
@@ -3770,7 +3896,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1039</v>
+        <v>1081</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3820,7 +3946,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1040</v>
+        <v>1082</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3838,7 +3964,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -3862,7 +3988,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1041</v>
+        <v>1083</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -3914,10 +4040,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1042</v>
+        <v>1084</v>
       </c>
       <c r="D5" t="s">
-        <v>1042</v>
+        <v>1084</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -3968,10 +4094,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1043</v>
+        <v>1085</v>
       </c>
       <c r="D6" t="s">
-        <v>1043</v>
+        <v>1085</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4026,10 +4152,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1044</v>
+        <v>1086</v>
       </c>
       <c r="D7" t="s">
-        <v>1044</v>
+        <v>1086</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4090,7 +4216,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1045</v>
+        <v>1087</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4146,7 +4272,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1046</v>
+        <v>1088</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -4186,7 +4312,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1047</v>
+        <v>1089</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4226,7 +4352,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1048</v>
+        <v>1090</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4266,7 +4392,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1049</v>
+        <v>1091</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4308,10 +4434,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1050</v>
+        <v>1092</v>
       </c>
       <c r="D13" t="s">
-        <v>1050</v>
+        <v>1092</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -4362,10 +4488,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1051</v>
+        <v>1093</v>
       </c>
       <c r="D14" t="s">
-        <v>1051</v>
+        <v>1093</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4416,10 +4542,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1052</v>
+        <v>1094</v>
       </c>
       <c r="D15" t="s">
-        <v>1052</v>
+        <v>1094</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4470,10 +4596,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1053</v>
+        <v>1095</v>
       </c>
       <c r="D16" t="s">
-        <v>1053</v>
+        <v>1095</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4524,10 +4650,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1054</v>
+        <v>1096</v>
       </c>
       <c r="D17" t="s">
-        <v>1054</v>
+        <v>1096</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4578,7 +4704,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1055</v>
+        <v>1097</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4620,7 +4746,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1056</v>
+        <v>1098</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4672,7 +4798,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1057</v>
+        <v>1099</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4724,7 +4850,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1058</v>
+        <v>1100</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4778,7 +4904,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1059</v>
+        <v>1101</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 4th july 2022
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5713" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5923" uniqueCount="1144">
   <si>
     <t>Sno</t>
   </si>
@@ -3320,6 +3320,132 @@
   </si>
   <si>
     <t>320018612539</t>
+  </si>
+  <si>
+    <t>320018614760</t>
+  </si>
+  <si>
+    <t>320018614770</t>
+  </si>
+  <si>
+    <t>320018614807</t>
+  </si>
+  <si>
+    <t>320018614829</t>
+  </si>
+  <si>
+    <t>320018614862</t>
+  </si>
+  <si>
+    <t>320018614884</t>
+  </si>
+  <si>
+    <t>320018614910</t>
+  </si>
+  <si>
+    <t>320018614932</t>
+  </si>
+  <si>
+    <t>320018614965</t>
+  </si>
+  <si>
+    <t>320018614987</t>
+  </si>
+  <si>
+    <t>320018615023</t>
+  </si>
+  <si>
+    <t>320018615045</t>
+  </si>
+  <si>
+    <t>320018615078</t>
+  </si>
+  <si>
+    <t>320018615090</t>
+  </si>
+  <si>
+    <t>320018615126</t>
+  </si>
+  <si>
+    <t>320018615148</t>
+  </si>
+  <si>
+    <t>320018615181</t>
+  </si>
+  <si>
+    <t>320018615207</t>
+  </si>
+  <si>
+    <t>320018615230</t>
+  </si>
+  <si>
+    <t>320018615251</t>
+  </si>
+  <si>
+    <t>320018615321</t>
+  </si>
+  <si>
+    <t>320018616270</t>
+  </si>
+  <si>
+    <t>320018616280</t>
+  </si>
+  <si>
+    <t>320018616317</t>
+  </si>
+  <si>
+    <t>320018616339</t>
+  </si>
+  <si>
+    <t>320018616372</t>
+  </si>
+  <si>
+    <t>320018616394</t>
+  </si>
+  <si>
+    <t>320018616420</t>
+  </si>
+  <si>
+    <t>320018616442</t>
+  </si>
+  <si>
+    <t>320018616475</t>
+  </si>
+  <si>
+    <t>320018616497</t>
+  </si>
+  <si>
+    <t>320018616534</t>
+  </si>
+  <si>
+    <t>320018616556</t>
+  </si>
+  <si>
+    <t>320018616589</t>
+  </si>
+  <si>
+    <t>320018616604</t>
+  </si>
+  <si>
+    <t>320018616637</t>
+  </si>
+  <si>
+    <t>320018616659</t>
+  </si>
+  <si>
+    <t>320018616692</t>
+  </si>
+  <si>
+    <t>320018616718</t>
+  </si>
+  <si>
+    <t>320018616740</t>
+  </si>
+  <si>
+    <t>320018616762</t>
+  </si>
+  <si>
+    <t>320018616795</t>
   </si>
 </sst>
 </file>
@@ -3896,7 +4022,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1081</v>
+        <v>1123</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -3946,7 +4072,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1082</v>
+        <v>1124</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -3988,7 +4114,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1083</v>
+        <v>1125</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4040,10 +4166,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1084</v>
+        <v>1126</v>
       </c>
       <c r="D5" t="s">
-        <v>1084</v>
+        <v>1126</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4094,10 +4220,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1085</v>
+        <v>1127</v>
       </c>
       <c r="D6" t="s">
-        <v>1085</v>
+        <v>1127</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4152,10 +4278,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1086</v>
+        <v>1128</v>
       </c>
       <c r="D7" t="s">
-        <v>1086</v>
+        <v>1128</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4216,7 +4342,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1087</v>
+        <v>1129</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4272,7 +4398,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1088</v>
+        <v>1130</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -4312,7 +4438,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1089</v>
+        <v>1131</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4352,7 +4478,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1090</v>
+        <v>1132</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4392,7 +4518,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1091</v>
+        <v>1133</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4434,10 +4560,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1092</v>
+        <v>1134</v>
       </c>
       <c r="D13" t="s">
-        <v>1092</v>
+        <v>1134</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -4488,10 +4614,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1093</v>
+        <v>1135</v>
       </c>
       <c r="D14" t="s">
-        <v>1093</v>
+        <v>1135</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4542,10 +4668,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1094</v>
+        <v>1136</v>
       </c>
       <c r="D15" t="s">
-        <v>1094</v>
+        <v>1136</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4596,10 +4722,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1095</v>
+        <v>1137</v>
       </c>
       <c r="D16" t="s">
-        <v>1095</v>
+        <v>1137</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4650,10 +4776,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1096</v>
+        <v>1138</v>
       </c>
       <c r="D17" t="s">
-        <v>1096</v>
+        <v>1138</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4704,7 +4830,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1097</v>
+        <v>1139</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4746,7 +4872,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1098</v>
+        <v>1140</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4798,7 +4924,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1099</v>
+        <v>1141</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4850,7 +4976,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1100</v>
+        <v>1142</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -4904,7 +5030,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1101</v>
+        <v>1143</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of cheetah and baseinit class
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5923" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6364" uniqueCount="1239">
   <si>
     <t>Sno</t>
   </si>
@@ -3446,6 +3446,291 @@
   </si>
   <si>
     <t>320018616795</t>
+  </si>
+  <si>
+    <t>320018625068</t>
+  </si>
+  <si>
+    <t>320018627152</t>
+  </si>
+  <si>
+    <t>320018627163</t>
+  </si>
+  <si>
+    <t>320018627196</t>
+  </si>
+  <si>
+    <t>320018627211</t>
+  </si>
+  <si>
+    <t>320018627255</t>
+  </si>
+  <si>
+    <t>320018627277</t>
+  </si>
+  <si>
+    <t>320018627303</t>
+  </si>
+  <si>
+    <t>320018627325</t>
+  </si>
+  <si>
+    <t>320018627358</t>
+  </si>
+  <si>
+    <t>320018627370</t>
+  </si>
+  <si>
+    <t>320018627417</t>
+  </si>
+  <si>
+    <t>320018627439</t>
+  </si>
+  <si>
+    <t>320018627461</t>
+  </si>
+  <si>
+    <t>320018627483</t>
+  </si>
+  <si>
+    <t>320018627510</t>
+  </si>
+  <si>
+    <t>320018627531</t>
+  </si>
+  <si>
+    <t>320018627575</t>
+  </si>
+  <si>
+    <t>320018627597</t>
+  </si>
+  <si>
+    <t>320018627623</t>
+  </si>
+  <si>
+    <t>320018627645</t>
+  </si>
+  <si>
+    <t>320018627678</t>
+  </si>
+  <si>
+    <t>320018628652</t>
+  </si>
+  <si>
+    <t>320018628696</t>
+  </si>
+  <si>
+    <t>320018628755</t>
+  </si>
+  <si>
+    <t>320018628777</t>
+  </si>
+  <si>
+    <t>320018628803</t>
+  </si>
+  <si>
+    <t>320018628858</t>
+  </si>
+  <si>
+    <t>320018628917</t>
+  </si>
+  <si>
+    <t>320018628939</t>
+  </si>
+  <si>
+    <t>320018628961</t>
+  </si>
+  <si>
+    <t>320018628983</t>
+  </si>
+  <si>
+    <t>320018629019</t>
+  </si>
+  <si>
+    <t>320018629030</t>
+  </si>
+  <si>
+    <t>320018629074</t>
+  </si>
+  <si>
+    <t>320018629096</t>
+  </si>
+  <si>
+    <t>320018629122</t>
+  </si>
+  <si>
+    <t>320018629144</t>
+  </si>
+  <si>
+    <t>320018629177</t>
+  </si>
+  <si>
+    <t>320018641400</t>
+  </si>
+  <si>
+    <t>320018641410</t>
+  </si>
+  <si>
+    <t>320018641443</t>
+  </si>
+  <si>
+    <t>320018641465</t>
+  </si>
+  <si>
+    <t>320018641502</t>
+  </si>
+  <si>
+    <t>320018641524</t>
+  </si>
+  <si>
+    <t>320018641557</t>
+  </si>
+  <si>
+    <t>320018641671</t>
+  </si>
+  <si>
+    <t>320018641708</t>
+  </si>
+  <si>
+    <t>320018641720</t>
+  </si>
+  <si>
+    <t>320018641763</t>
+  </si>
+  <si>
+    <t>320018641785</t>
+  </si>
+  <si>
+    <t>320018641811</t>
+  </si>
+  <si>
+    <t>320018641833</t>
+  </si>
+  <si>
+    <t>320018641866</t>
+  </si>
+  <si>
+    <t>320018641888</t>
+  </si>
+  <si>
+    <t>320018641925</t>
+  </si>
+  <si>
+    <t>320018641947</t>
+  </si>
+  <si>
+    <t>320018641970</t>
+  </si>
+  <si>
+    <t>320018641991</t>
+  </si>
+  <si>
+    <t>320018642027</t>
+  </si>
+  <si>
+    <t>320018645471</t>
+  </si>
+  <si>
+    <t>320018645482</t>
+  </si>
+  <si>
+    <t>320018645519</t>
+  </si>
+  <si>
+    <t>320018645530</t>
+  </si>
+  <si>
+    <t>320018645574</t>
+  </si>
+  <si>
+    <t>320018645596</t>
+  </si>
+  <si>
+    <t>320018645622</t>
+  </si>
+  <si>
+    <t>320018645644</t>
+  </si>
+  <si>
+    <t>320018645677</t>
+  </si>
+  <si>
+    <t>320018645699</t>
+  </si>
+  <si>
+    <t>320018645736</t>
+  </si>
+  <si>
+    <t>320018645758</t>
+  </si>
+  <si>
+    <t>320018645780</t>
+  </si>
+  <si>
+    <t>320018645806</t>
+  </si>
+  <si>
+    <t>320018645839</t>
+  </si>
+  <si>
+    <t>320018645850</t>
+  </si>
+  <si>
+    <t>320018645894</t>
+  </si>
+  <si>
+    <t>320018645910</t>
+  </si>
+  <si>
+    <t>320018645942</t>
+  </si>
+  <si>
+    <t>320018645964</t>
+  </si>
+  <si>
+    <t>320018645997</t>
+  </si>
+  <si>
+    <t>320018655634</t>
+  </si>
+  <si>
+    <t>320018655645</t>
+  </si>
+  <si>
+    <t>320018655678</t>
+  </si>
+  <si>
+    <t>320018655690</t>
+  </si>
+  <si>
+    <t>320018655760</t>
+  </si>
+  <si>
+    <t>320018655781</t>
+  </si>
+  <si>
+    <t>320018655818</t>
+  </si>
+  <si>
+    <t>320018655830</t>
+  </si>
+  <si>
+    <t>320018655862</t>
+  </si>
+  <si>
+    <t>320018655884</t>
+  </si>
+  <si>
+    <t>320018655921</t>
+  </si>
+  <si>
+    <t>320018655943</t>
+  </si>
+  <si>
+    <t>320018655976</t>
+  </si>
+  <si>
+    <t>320018655998</t>
   </si>
 </sst>
 </file>
@@ -4022,7 +4307,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1123</v>
+        <v>1225</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -4072,7 +4357,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1124</v>
+        <v>1226</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -4114,7 +4399,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1125</v>
+        <v>1227</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4166,10 +4451,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1126</v>
+        <v>1228</v>
       </c>
       <c r="D5" t="s">
-        <v>1126</v>
+        <v>1228</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4220,10 +4505,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1127</v>
+        <v>1229</v>
       </c>
       <c r="D6" t="s">
-        <v>1127</v>
+        <v>1229</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4278,10 +4563,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1128</v>
+        <v>1230</v>
       </c>
       <c r="D7" t="s">
-        <v>1128</v>
+        <v>1230</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4342,7 +4627,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1129</v>
+        <v>1231</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4398,7 +4683,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1130</v>
+        <v>1232</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -4438,7 +4723,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1131</v>
+        <v>1233</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4478,7 +4763,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1132</v>
+        <v>1234</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4518,7 +4803,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1133</v>
+        <v>1235</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4560,10 +4845,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1134</v>
+        <v>1236</v>
       </c>
       <c r="D13" t="s">
-        <v>1134</v>
+        <v>1236</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -4614,10 +4899,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1135</v>
+        <v>1237</v>
       </c>
       <c r="D14" t="s">
-        <v>1135</v>
+        <v>1237</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4668,10 +4953,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1136</v>
+        <v>1238</v>
       </c>
       <c r="D15" t="s">
-        <v>1136</v>
+        <v>1238</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -4722,10 +5007,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1137</v>
+        <v>1218</v>
       </c>
       <c r="D16" t="s">
-        <v>1137</v>
+        <v>1218</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -4776,10 +5061,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1138</v>
+        <v>1219</v>
       </c>
       <c r="D17" t="s">
-        <v>1138</v>
+        <v>1219</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -4830,7 +5115,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1139</v>
+        <v>1220</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -4872,7 +5157,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1140</v>
+        <v>1221</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -4924,7 +5209,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1141</v>
+        <v>1222</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -4976,7 +5261,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1142</v>
+        <v>1223</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -5030,7 +5315,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1143</v>
+        <v>1224</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 11th July 2022
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6364" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6572" uniqueCount="1277">
   <si>
     <t>Sno</t>
   </si>
@@ -3731,6 +3731,120 @@
   </si>
   <si>
     <t>320018655998</t>
+  </si>
+  <si>
+    <t>320018656300</t>
+  </si>
+  <si>
+    <t>320018656310</t>
+  </si>
+  <si>
+    <t>320018656343</t>
+  </si>
+  <si>
+    <t>320018657913</t>
+  </si>
+  <si>
+    <t>320018657957</t>
+  </si>
+  <si>
+    <t>320018657979</t>
+  </si>
+  <si>
+    <t>320018658004</t>
+  </si>
+  <si>
+    <t>320018658026</t>
+  </si>
+  <si>
+    <t>320018658059</t>
+  </si>
+  <si>
+    <t>320018658070</t>
+  </si>
+  <si>
+    <t>320018658129</t>
+  </si>
+  <si>
+    <t>320018658140</t>
+  </si>
+  <si>
+    <t>320018658173</t>
+  </si>
+  <si>
+    <t>320018658195</t>
+  </si>
+  <si>
+    <t>320018658221</t>
+  </si>
+  <si>
+    <t>320018658243</t>
+  </si>
+  <si>
+    <t>320018675544</t>
+  </si>
+  <si>
+    <t>320018675783</t>
+  </si>
+  <si>
+    <t>320018675794</t>
+  </si>
+  <si>
+    <t>320018675820</t>
+  </si>
+  <si>
+    <t>320018675842</t>
+  </si>
+  <si>
+    <t>320018675886</t>
+  </si>
+  <si>
+    <t>320018675901</t>
+  </si>
+  <si>
+    <t>320018675934</t>
+  </si>
+  <si>
+    <t>320018675956</t>
+  </si>
+  <si>
+    <t>320018675989</t>
+  </si>
+  <si>
+    <t>320018676025</t>
+  </si>
+  <si>
+    <t>320018676069</t>
+  </si>
+  <si>
+    <t>320018676080</t>
+  </si>
+  <si>
+    <t>320018676117</t>
+  </si>
+  <si>
+    <t>320018676139</t>
+  </si>
+  <si>
+    <t>320018676161</t>
+  </si>
+  <si>
+    <t>320018676183</t>
+  </si>
+  <si>
+    <t>320018677775</t>
+  </si>
+  <si>
+    <t>320018677797</t>
+  </si>
+  <si>
+    <t>320018677948</t>
+  </si>
+  <si>
+    <t>320018677992</t>
+  </si>
+  <si>
+    <t>320018678028</t>
   </si>
 </sst>
 </file>
@@ -4307,7 +4421,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1225</v>
+        <v>1256</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -4357,7 +4471,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1226</v>
+        <v>1257</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -4375,7 +4489,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -4399,7 +4513,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1227</v>
+        <v>1258</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4451,10 +4565,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1228</v>
+        <v>1259</v>
       </c>
       <c r="D5" t="s">
-        <v>1228</v>
+        <v>1259</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4505,10 +4619,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1229</v>
+        <v>1260</v>
       </c>
       <c r="D6" t="s">
-        <v>1229</v>
+        <v>1260</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4563,10 +4677,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1230</v>
+        <v>1261</v>
       </c>
       <c r="D7" t="s">
-        <v>1230</v>
+        <v>1261</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4627,7 +4741,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1231</v>
+        <v>1262</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4683,7 +4797,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1232</v>
+        <v>1263</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -4723,7 +4837,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1233</v>
+        <v>1264</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4763,7 +4877,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1234</v>
+        <v>1265</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4803,7 +4917,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1235</v>
+        <v>1266</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4845,10 +4959,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1236</v>
+        <v>1267</v>
       </c>
       <c r="D13" t="s">
-        <v>1236</v>
+        <v>1267</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -4899,10 +5013,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1237</v>
+        <v>1268</v>
       </c>
       <c r="D14" t="s">
-        <v>1237</v>
+        <v>1268</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -4953,10 +5067,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1238</v>
+        <v>1269</v>
       </c>
       <c r="D15" t="s">
-        <v>1238</v>
+        <v>1269</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -5007,10 +5121,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1218</v>
+        <v>1270</v>
       </c>
       <c r="D16" t="s">
-        <v>1218</v>
+        <v>1270</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -5061,10 +5175,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1219</v>
+        <v>1271</v>
       </c>
       <c r="D17" t="s">
-        <v>1219</v>
+        <v>1271</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -5115,7 +5229,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1220</v>
+        <v>1272</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -5157,7 +5271,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1221</v>
+        <v>1273</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -5209,7 +5323,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1222</v>
+        <v>1274</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -5261,7 +5375,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1223</v>
+        <v>1275</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -5315,7 +5429,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1224</v>
+        <v>1276</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of Login email on 12th July 2022
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6572" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6594" uniqueCount="1291">
   <si>
     <t>Sno</t>
   </si>
@@ -3845,6 +3845,48 @@
   </si>
   <si>
     <t>320018678028</t>
+  </si>
+  <si>
+    <t>320018680212</t>
+  </si>
+  <si>
+    <t>320018680223</t>
+  </si>
+  <si>
+    <t>320018680256</t>
+  </si>
+  <si>
+    <t>320018680315</t>
+  </si>
+  <si>
+    <t>320018680337</t>
+  </si>
+  <si>
+    <t>320018680360</t>
+  </si>
+  <si>
+    <t>320018680381</t>
+  </si>
+  <si>
+    <t>320018680418</t>
+  </si>
+  <si>
+    <t>320018680430</t>
+  </si>
+  <si>
+    <t>320018680473</t>
+  </si>
+  <si>
+    <t>320018680495</t>
+  </si>
+  <si>
+    <t>320018680521</t>
+  </si>
+  <si>
+    <t>320018680543</t>
+  </si>
+  <si>
+    <t>320018680576</t>
   </si>
 </sst>
 </file>
@@ -4421,7 +4463,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1256</v>
+        <v>1277</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -4471,7 +4513,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1257</v>
+        <v>1278</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -4513,7 +4555,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1258</v>
+        <v>1279</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4565,10 +4607,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1259</v>
+        <v>559</v>
       </c>
       <c r="D5" t="s">
-        <v>1259</v>
+        <v>559</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4619,10 +4661,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1260</v>
+        <v>1280</v>
       </c>
       <c r="D6" t="s">
-        <v>1260</v>
+        <v>1280</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4677,10 +4719,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1261</v>
+        <v>1281</v>
       </c>
       <c r="D7" t="s">
-        <v>1261</v>
+        <v>1281</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4741,7 +4783,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1262</v>
+        <v>1282</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4797,7 +4839,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1263</v>
+        <v>1283</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -4837,7 +4879,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1264</v>
+        <v>1284</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -4877,7 +4919,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1265</v>
+        <v>1285</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -4917,7 +4959,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1266</v>
+        <v>1286</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -4959,10 +5001,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1267</v>
+        <v>1287</v>
       </c>
       <c r="D13" t="s">
-        <v>1267</v>
+        <v>1287</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -5013,10 +5055,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1268</v>
+        <v>1288</v>
       </c>
       <c r="D14" t="s">
-        <v>1268</v>
+        <v>1288</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -5067,10 +5109,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1269</v>
+        <v>1289</v>
       </c>
       <c r="D15" t="s">
-        <v>1269</v>
+        <v>1289</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -5121,10 +5163,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1270</v>
+        <v>1290</v>
       </c>
       <c r="D16" t="s">
-        <v>1270</v>
+        <v>1290</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">

</xml_diff>

<commit_message>
Changes of 15th july 2022
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6890" uniqueCount="1339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6996" uniqueCount="1360">
   <si>
     <t>Sno</t>
   </si>
@@ -4031,6 +4031,69 @@
   </si>
   <si>
     <t>320018697685</t>
+  </si>
+  <si>
+    <t>320018701475</t>
+  </si>
+  <si>
+    <t>320018701497</t>
+  </si>
+  <si>
+    <t>320018701523</t>
+  </si>
+  <si>
+    <t>320018701545</t>
+  </si>
+  <si>
+    <t>320018701589</t>
+  </si>
+  <si>
+    <t>320018701604</t>
+  </si>
+  <si>
+    <t>320018701648</t>
+  </si>
+  <si>
+    <t>320018702081</t>
+  </si>
+  <si>
+    <t>320018702130</t>
+  </si>
+  <si>
+    <t>320018702162</t>
+  </si>
+  <si>
+    <t>320018702210</t>
+  </si>
+  <si>
+    <t>320018702232</t>
+  </si>
+  <si>
+    <t>320018702265</t>
+  </si>
+  <si>
+    <t>320018702287</t>
+  </si>
+  <si>
+    <t>320018702324</t>
+  </si>
+  <si>
+    <t>320018702368</t>
+  </si>
+  <si>
+    <t>320018702405</t>
+  </si>
+  <si>
+    <t>320018702427</t>
+  </si>
+  <si>
+    <t>320018702450</t>
+  </si>
+  <si>
+    <t>320018702471</t>
+  </si>
+  <si>
+    <t>320018702508</t>
   </si>
 </sst>
 </file>
@@ -4607,7 +4670,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1318</v>
+        <v>1339</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -4657,7 +4720,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1319</v>
+        <v>1340</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -4699,7 +4762,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1320</v>
+        <v>1341</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4751,10 +4814,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1321</v>
+        <v>1342</v>
       </c>
       <c r="D5" t="s">
-        <v>1321</v>
+        <v>1342</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4805,10 +4868,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1322</v>
+        <v>1343</v>
       </c>
       <c r="D6" t="s">
-        <v>1322</v>
+        <v>1343</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4863,10 +4926,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1323</v>
+        <v>1344</v>
       </c>
       <c r="D7" t="s">
-        <v>1323</v>
+        <v>1344</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4927,7 +4990,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1324</v>
+        <v>1345</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -4983,7 +5046,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1325</v>
+        <v>1346</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -5023,7 +5086,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1326</v>
+        <v>1347</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -5063,7 +5126,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1327</v>
+        <v>1348</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -5103,7 +5166,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1328</v>
+        <v>1349</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -5145,10 +5208,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1329</v>
+        <v>1350</v>
       </c>
       <c r="D13" t="s">
-        <v>1329</v>
+        <v>1350</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -5199,10 +5262,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1330</v>
+        <v>1351</v>
       </c>
       <c r="D14" t="s">
-        <v>1330</v>
+        <v>1351</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -5253,10 +5316,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1331</v>
+        <v>1352</v>
       </c>
       <c r="D15" t="s">
-        <v>1331</v>
+        <v>1352</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -5307,10 +5370,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1332</v>
+        <v>1353</v>
       </c>
       <c r="D16" t="s">
-        <v>1332</v>
+        <v>1353</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -5361,10 +5424,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1333</v>
+        <v>1354</v>
       </c>
       <c r="D17" t="s">
-        <v>1333</v>
+        <v>1354</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -5415,7 +5478,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1334</v>
+        <v>1355</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -5457,7 +5520,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1335</v>
+        <v>1356</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -5509,7 +5572,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1336</v>
+        <v>1357</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -5561,7 +5624,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1337</v>
+        <v>1358</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -5615,7 +5678,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1338</v>
+        <v>1359</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of Rate Verification
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6996" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7102" uniqueCount="1381">
   <si>
     <t>Sno</t>
   </si>
@@ -4094,6 +4094,69 @@
   </si>
   <si>
     <t>320018702508</t>
+  </si>
+  <si>
+    <t>320018714339</t>
+  </si>
+  <si>
+    <t>320018714340</t>
+  </si>
+  <si>
+    <t>320018714372</t>
+  </si>
+  <si>
+    <t>320018714394</t>
+  </si>
+  <si>
+    <t>320018714431</t>
+  </si>
+  <si>
+    <t>320018714453</t>
+  </si>
+  <si>
+    <t>320018714486</t>
+  </si>
+  <si>
+    <t>320018714501</t>
+  </si>
+  <si>
+    <t>320018714534</t>
+  </si>
+  <si>
+    <t>320018714556</t>
+  </si>
+  <si>
+    <t>320018714590</t>
+  </si>
+  <si>
+    <t>320018714615</t>
+  </si>
+  <si>
+    <t>320018714648</t>
+  </si>
+  <si>
+    <t>320018714660</t>
+  </si>
+  <si>
+    <t>320018714692</t>
+  </si>
+  <si>
+    <t>320018714718</t>
+  </si>
+  <si>
+    <t>320018714751</t>
+  </si>
+  <si>
+    <t>320018714773</t>
+  </si>
+  <si>
+    <t>320018714800</t>
+  </si>
+  <si>
+    <t>320018714821</t>
+  </si>
+  <si>
+    <t>320018714854</t>
   </si>
 </sst>
 </file>
@@ -4670,7 +4733,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1339</v>
+        <v>1360</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -4720,7 +4783,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1340</v>
+        <v>1361</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -4762,7 +4825,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1341</v>
+        <v>1362</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4814,10 +4877,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1342</v>
+        <v>1363</v>
       </c>
       <c r="D5" t="s">
-        <v>1342</v>
+        <v>1363</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4868,10 +4931,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1343</v>
+        <v>1364</v>
       </c>
       <c r="D6" t="s">
-        <v>1343</v>
+        <v>1364</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4926,10 +4989,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1344</v>
+        <v>1365</v>
       </c>
       <c r="D7" t="s">
-        <v>1344</v>
+        <v>1365</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -4990,7 +5053,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1345</v>
+        <v>1366</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -5046,7 +5109,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1346</v>
+        <v>1367</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -5086,7 +5149,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1347</v>
+        <v>1368</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -5126,7 +5189,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1348</v>
+        <v>1369</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -5166,7 +5229,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1349</v>
+        <v>1370</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -5208,10 +5271,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1350</v>
+        <v>1371</v>
       </c>
       <c r="D13" t="s">
-        <v>1350</v>
+        <v>1371</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -5262,10 +5325,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1351</v>
+        <v>1372</v>
       </c>
       <c r="D14" t="s">
-        <v>1351</v>
+        <v>1372</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -5316,10 +5379,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1352</v>
+        <v>1373</v>
       </c>
       <c r="D15" t="s">
-        <v>1352</v>
+        <v>1373</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -5370,10 +5433,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1353</v>
+        <v>1374</v>
       </c>
       <c r="D16" t="s">
-        <v>1353</v>
+        <v>1374</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -5424,10 +5487,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1354</v>
+        <v>1375</v>
       </c>
       <c r="D17" t="s">
-        <v>1354</v>
+        <v>1375</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -5478,7 +5541,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1355</v>
+        <v>1376</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -5520,7 +5583,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1356</v>
+        <v>1377</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -5572,7 +5635,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1357</v>
+        <v>1378</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -5624,7 +5687,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1358</v>
+        <v>1379</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -5678,7 +5741,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1359</v>
+        <v>1380</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Added 1 more charge in SHipment Creation
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7102" uniqueCount="1381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7309" uniqueCount="1462">
   <si>
     <t>Sno</t>
   </si>
@@ -4157,6 +4157,249 @@
   </si>
   <si>
     <t>320018714854</t>
+  </si>
+  <si>
+    <t>320018720172</t>
+  </si>
+  <si>
+    <t>320018720301</t>
+  </si>
+  <si>
+    <t>320018720312</t>
+  </si>
+  <si>
+    <t>320018720345</t>
+  </si>
+  <si>
+    <t>320018720367</t>
+  </si>
+  <si>
+    <t>320018720404</t>
+  </si>
+  <si>
+    <t>320018720437</t>
+  </si>
+  <si>
+    <t>320018720460</t>
+  </si>
+  <si>
+    <t>320018720481</t>
+  </si>
+  <si>
+    <t>320018720518</t>
+  </si>
+  <si>
+    <t>320018720530</t>
+  </si>
+  <si>
+    <t>320018720573</t>
+  </si>
+  <si>
+    <t>320018720600</t>
+  </si>
+  <si>
+    <t>320018720610</t>
+  </si>
+  <si>
+    <t>320018720643</t>
+  </si>
+  <si>
+    <t>320018720665</t>
+  </si>
+  <si>
+    <t>320018720702</t>
+  </si>
+  <si>
+    <t>320018720713</t>
+  </si>
+  <si>
+    <t>320018720746</t>
+  </si>
+  <si>
+    <t>320018720768</t>
+  </si>
+  <si>
+    <t>320018720816</t>
+  </si>
+  <si>
+    <t>320018720838</t>
+  </si>
+  <si>
+    <t>320018720860</t>
+  </si>
+  <si>
+    <t>320018720882</t>
+  </si>
+  <si>
+    <t>320018720919</t>
+  </si>
+  <si>
+    <t>320018720930</t>
+  </si>
+  <si>
+    <t>320018720974</t>
+  </si>
+  <si>
+    <t>320018720996</t>
+  </si>
+  <si>
+    <t>320018721032</t>
+  </si>
+  <si>
+    <t>320018721054</t>
+  </si>
+  <si>
+    <t>320018721065</t>
+  </si>
+  <si>
+    <t>320018721098</t>
+  </si>
+  <si>
+    <t>320018721113</t>
+  </si>
+  <si>
+    <t>320018721157</t>
+  </si>
+  <si>
+    <t>320018721179</t>
+  </si>
+  <si>
+    <t>320018721282</t>
+  </si>
+  <si>
+    <t>320018721308</t>
+  </si>
+  <si>
+    <t>320018721341</t>
+  </si>
+  <si>
+    <t>320018721374</t>
+  </si>
+  <si>
+    <t>320018721411</t>
+  </si>
+  <si>
+    <t>320018721422</t>
+  </si>
+  <si>
+    <t>320018721455</t>
+  </si>
+  <si>
+    <t>320018721477</t>
+  </si>
+  <si>
+    <t>320018721525</t>
+  </si>
+  <si>
+    <t>320018721547</t>
+  </si>
+  <si>
+    <t>320018721570</t>
+  </si>
+  <si>
+    <t>320018721591</t>
+  </si>
+  <si>
+    <t>320018721628</t>
+  </si>
+  <si>
+    <t>320018721640</t>
+  </si>
+  <si>
+    <t>320018721683</t>
+  </si>
+  <si>
+    <t>320018721709</t>
+  </si>
+  <si>
+    <t>320018721731</t>
+  </si>
+  <si>
+    <t>320018721753</t>
+  </si>
+  <si>
+    <t>320018721786</t>
+  </si>
+  <si>
+    <t>320018721801</t>
+  </si>
+  <si>
+    <t>320018721845</t>
+  </si>
+  <si>
+    <t>320018721867</t>
+  </si>
+  <si>
+    <t>320018721926</t>
+  </si>
+  <si>
+    <t>320018721948</t>
+  </si>
+  <si>
+    <t>320018721970</t>
+  </si>
+  <si>
+    <t>320018722164</t>
+  </si>
+  <si>
+    <t>320018722370</t>
+  </si>
+  <si>
+    <t>320018722429</t>
+  </si>
+  <si>
+    <t>320018722440</t>
+  </si>
+  <si>
+    <t>320018722484</t>
+  </si>
+  <si>
+    <t>320018722510</t>
+  </si>
+  <si>
+    <t>320018722543</t>
+  </si>
+  <si>
+    <t>320018722565</t>
+  </si>
+  <si>
+    <t>320018722602</t>
+  </si>
+  <si>
+    <t>320018722646</t>
+  </si>
+  <si>
+    <t>320018722680</t>
+  </si>
+  <si>
+    <t>320018722716</t>
+  </si>
+  <si>
+    <t>320018722749</t>
+  </si>
+  <si>
+    <t>320018722782</t>
+  </si>
+  <si>
+    <t>320018722819</t>
+  </si>
+  <si>
+    <t>320018722830</t>
+  </si>
+  <si>
+    <t>320018722874</t>
+  </si>
+  <si>
+    <t>320018722896</t>
+  </si>
+  <si>
+    <t>320018722922</t>
+  </si>
+  <si>
+    <t>320018722944</t>
+  </si>
+  <si>
+    <t>320018722977</t>
   </si>
 </sst>
 </file>
@@ -4733,7 +4976,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1360</v>
+        <v>1441</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -4783,7 +5026,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1361</v>
+        <v>1442</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -4825,7 +5068,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1362</v>
+        <v>1443</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -4877,10 +5120,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1363</v>
+        <v>1444</v>
       </c>
       <c r="D5" t="s">
-        <v>1363</v>
+        <v>1444</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4931,10 +5174,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1364</v>
+        <v>1445</v>
       </c>
       <c r="D6" t="s">
-        <v>1364</v>
+        <v>1445</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -4989,10 +5232,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1365</v>
+        <v>1446</v>
       </c>
       <c r="D7" t="s">
-        <v>1365</v>
+        <v>1446</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -5053,7 +5296,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1366</v>
+        <v>1447</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -5109,7 +5352,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1367</v>
+        <v>1448</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -5149,7 +5392,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1368</v>
+        <v>1449</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -5189,7 +5432,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1369</v>
+        <v>1450</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -5229,7 +5472,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1370</v>
+        <v>1451</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -5271,10 +5514,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1371</v>
+        <v>1452</v>
       </c>
       <c r="D13" t="s">
-        <v>1371</v>
+        <v>1452</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -5325,10 +5568,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1372</v>
+        <v>1453</v>
       </c>
       <c r="D14" t="s">
-        <v>1372</v>
+        <v>1453</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -5379,10 +5622,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1373</v>
+        <v>1454</v>
       </c>
       <c r="D15" t="s">
-        <v>1373</v>
+        <v>1454</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -5433,10 +5676,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1374</v>
+        <v>1455</v>
       </c>
       <c r="D16" t="s">
-        <v>1374</v>
+        <v>1455</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -5487,10 +5730,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1375</v>
+        <v>1456</v>
       </c>
       <c r="D17" t="s">
-        <v>1375</v>
+        <v>1456</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -5541,7 +5784,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1376</v>
+        <v>1457</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -5583,7 +5826,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1377</v>
+        <v>1458</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -5635,7 +5878,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1378</v>
+        <v>1459</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -5687,7 +5930,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1379</v>
+        <v>1460</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -5741,7 +5984,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1380</v>
+        <v>1461</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 26th july 2022
</commit_message>
<xml_diff>
--- a/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplicationMaven/src/main/resources/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7309" uniqueCount="1462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7415" uniqueCount="1483">
   <si>
     <t>Sno</t>
   </si>
@@ -4400,6 +4400,69 @@
   </si>
   <si>
     <t>320018722977</t>
+  </si>
+  <si>
+    <t>320018728611</t>
+  </si>
+  <si>
+    <t>320018728622</t>
+  </si>
+  <si>
+    <t>320018728655</t>
+  </si>
+  <si>
+    <t>320018728677</t>
+  </si>
+  <si>
+    <t>320018728714</t>
+  </si>
+  <si>
+    <t>320018728736</t>
+  </si>
+  <si>
+    <t>320018728770</t>
+  </si>
+  <si>
+    <t>320018728791</t>
+  </si>
+  <si>
+    <t>320018728840</t>
+  </si>
+  <si>
+    <t>320018728861</t>
+  </si>
+  <si>
+    <t>320018728909</t>
+  </si>
+  <si>
+    <t>320018728931</t>
+  </si>
+  <si>
+    <t>320018728975</t>
+  </si>
+  <si>
+    <t>320018729011</t>
+  </si>
+  <si>
+    <t>320018729044</t>
+  </si>
+  <si>
+    <t>320018729066</t>
+  </si>
+  <si>
+    <t>320018729103</t>
+  </si>
+  <si>
+    <t>320018729136</t>
+  </si>
+  <si>
+    <t>320018729170</t>
+  </si>
+  <si>
+    <t>320018729191</t>
+  </si>
+  <si>
+    <t>320018729228</t>
   </si>
 </sst>
 </file>
@@ -4976,7 +5039,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1441</v>
+        <v>1462</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -5026,7 +5089,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>1442</v>
+        <v>1463</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -5068,7 +5131,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1443</v>
+        <v>1464</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -5120,10 +5183,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1444</v>
+        <v>1465</v>
       </c>
       <c r="D5" t="s">
-        <v>1444</v>
+        <v>1465</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -5174,10 +5237,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>1445</v>
+        <v>1466</v>
       </c>
       <c r="D6" t="s">
-        <v>1445</v>
+        <v>1466</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -5232,10 +5295,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>1446</v>
+        <v>1467</v>
       </c>
       <c r="D7" t="s">
-        <v>1446</v>
+        <v>1467</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -5296,7 +5359,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>1447</v>
+        <v>1468</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -5352,7 +5415,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>1448</v>
+        <v>1469</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -5392,7 +5455,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>1449</v>
+        <v>1470</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -5432,7 +5495,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1450</v>
+        <v>1471</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -5472,7 +5535,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>1451</v>
+        <v>1472</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -5514,10 +5577,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>1452</v>
+        <v>1473</v>
       </c>
       <c r="D13" t="s">
-        <v>1452</v>
+        <v>1473</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -5568,10 +5631,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>1453</v>
+        <v>1474</v>
       </c>
       <c r="D14" t="s">
-        <v>1453</v>
+        <v>1474</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -5622,10 +5685,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>1454</v>
+        <v>1475</v>
       </c>
       <c r="D15" t="s">
-        <v>1454</v>
+        <v>1475</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -5676,10 +5739,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>1455</v>
+        <v>1476</v>
       </c>
       <c r="D16" t="s">
-        <v>1455</v>
+        <v>1476</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -5730,10 +5793,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>1456</v>
+        <v>1477</v>
       </c>
       <c r="D17" t="s">
-        <v>1456</v>
+        <v>1477</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -5784,7 +5847,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>1457</v>
+        <v>1478</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -5826,7 +5889,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>1458</v>
+        <v>1479</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -5878,7 +5941,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>1459</v>
+        <v>1480</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -5930,7 +5993,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>1460</v>
+        <v>1481</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -5984,7 +6047,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>1461</v>
+        <v>1482</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>